<commit_message>
infographic alt text and exploratory weight
</commit_message>
<xml_diff>
--- a/code/significance_testing/exploratory_analysis/inputs/var read across - time series.XLSX
+++ b/code/significance_testing/exploratory_analysis/inputs/var read across - time series.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1251607\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2337714\Documents\R\71-ssb-pcos\code\significance_testing\exploratory_analysis\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8393E94B-95A0-4C74-8D28-B1FCBD17F4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2E2304-00F9-47C9-AD6E-C1343B191A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{369C3F55-ED05-41A1-A5DF-7D9D865E9E0E}"/>
+    <workbookView xWindow="28110" yWindow="0" windowWidth="23595" windowHeight="20985" activeTab="1" xr2:uid="{369C3F55-ED05-41A1-A5DF-7D9D865E9E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="68">
   <si>
     <t>PCOS4</t>
   </si>
@@ -249,7 +249,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,12 +390,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -785,10 +779,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1189,12 +1183,12 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9">
         <v>2009</v>
       </c>
@@ -1205,7 +1199,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>2010</v>
       </c>
@@ -1216,7 +1210,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2012</v>
       </c>
@@ -1224,7 +1218,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2014</v>
       </c>
@@ -1232,7 +1226,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2016</v>
       </c>
@@ -1240,7 +1234,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>2018</v>
       </c>
@@ -1248,7 +1242,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>2019</v>
       </c>
@@ -1256,7 +1250,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2020</v>
       </c>
@@ -1264,7 +1258,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>2021</v>
       </c>
@@ -1272,7 +1266,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>2022</v>
       </c>
@@ -1289,21 +1283,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A829DFF2-EC61-4116-8FF7-0FB7991EF5DC}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" customWidth="1"/>
+    <col min="1" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9">
         <v>2009</v>
       </c>
@@ -1335,7 +1329,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1391,7 +1385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1415,7 +1409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1439,7 +1433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1463,7 +1457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1487,7 +1481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1509,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1533,7 +1527,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1557,7 +1551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +1583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1613,7 +1607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1637,7 +1631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1661,7 +1655,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1685,7 +1679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1707,7 +1701,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1731,7 +1725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1755,7 +1749,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1779,7 +1773,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1797,7 +1791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1815,7 +1809,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1833,7 +1827,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1851,7 +1845,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1869,7 +1863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1887,7 +1881,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1905,7 +1899,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1923,7 +1917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1941,7 +1935,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1959,7 +1953,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1977,7 +1971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1995,7 +1989,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2013,7 +2007,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2031,7 +2025,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2049,7 +2043,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2067,7 +2061,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2085,7 +2079,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2103,7 +2097,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="4" t="s">
         <v>43</v>
       </c>
@@ -2129,7 +2123,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="4" t="s">
         <v>46</v>
       </c>
@@ -2153,7 +2147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="4" t="s">
         <v>49</v>
       </c>
@@ -2179,10 +2173,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="F41" t="s">
         <v>51</v>
       </c>
@@ -2199,17 +2199,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="F42" t="s">
         <v>53</v>
       </c>
       <c r="G42" t="s">
         <v>53</v>
       </c>
-      <c r="H42" s="6"/>
+      <c r="H42" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="I42" t="s">
         <v>53</v>
       </c>
@@ -2217,7 +2225,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
         <v>54</v>
       </c>
@@ -2244,7 +2252,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>